<commit_message>
bypass when center has no info
</commit_message>
<xml_diff>
--- a/resources/Senhas_v2.xlsx
+++ b/resources/Senhas_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\aee_digital_front\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5F22A8-57D4-4F37-AC21-C905B53AE6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59EB8DB-B39C-4106-AB83-1FF93BDC0973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5446,7 +5446,7 @@
   <dimension ref="A1:F366"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="F237" sqref="F237"/>
+      <selection activeCell="D245" sqref="D245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>